<commit_message>
add mean, median, stdev and write_csv
</commit_message>
<xml_diff>
--- a/samples/index_sample1.xlsx
+++ b/samples/index_sample1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\stock_analysis\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Git\git\stock_analysis\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Wind资讯" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>数据来源：Wind资讯</t>
   </si>
@@ -57,12 +57,24 @@
   </si>
   <si>
     <t>CSI300-Chuang Ye Ban</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>stdev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-m\-d;@"/>
   </numFmts>
@@ -472,13 +484,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,9 +505,10 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -529,8 +542,11 @@
       <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>40319</v>
       </c>
@@ -547,7 +563,7 @@
         <v>40319</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>40322</v>
       </c>
@@ -572,7 +588,7 @@
         <v>4.5473252837181732</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>40323</v>
       </c>
@@ -597,7 +613,7 @@
         <v>-0.72369800529702433</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>40324</v>
       </c>
@@ -622,7 +638,7 @@
         <v>0.27377335456555407</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>40325</v>
       </c>
@@ -650,7 +666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>40326</v>
       </c>
@@ -679,7 +695,7 @@
         <v>0.97817900521976497</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>40329</v>
       </c>
@@ -708,7 +724,7 @@
         <v>0.9329039678074752</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>40330</v>
       </c>
@@ -741,7 +757,7 @@
         <v>0.96112121902601555</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>40331</v>
       </c>
@@ -774,7 +790,7 @@
         <v>0.95402891781400923</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>40332</v>
       </c>
@@ -807,7 +823,7 @@
         <v>0.95593461729583151</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>40333</v>
       </c>
@@ -845,8 +861,17 @@
       <c r="N12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>40336</v>
       </c>
@@ -886,8 +911,20 @@
         <f>CORREL(H9:H13,J9:J13)</f>
         <v>0.14379675287497323</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <f>AVERAGE(L13:N13)</f>
+        <v>0.54643793232924376</v>
+      </c>
+      <c r="Q13">
+        <f>MEDIAN(L13:N13)</f>
+        <v>0.73515439581686282</v>
+      </c>
+      <c r="R13">
+        <f>_xlfn.STDEV.S(L13:N13)</f>
+        <v>0.34892521196168402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>40337</v>
       </c>
@@ -927,8 +964,20 @@
         <f t="shared" ref="N14:N16" si="3">CORREL(H10:H14,J10:J14)</f>
         <v>-0.31586058774763115</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <f t="shared" ref="P14:P16" si="4">AVERAGE(L14:N14)</f>
+        <v>0.19518936041915061</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ref="Q14:Q16" si="5">MEDIAN(L14:N14)</f>
+        <v>3.6280970509975655E-2</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ref="R14:R16" si="6">_xlfn.STDEV.S(L14:N14)</f>
+        <v>0.60632833541831721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>40338</v>
       </c>
@@ -968,8 +1017,20 @@
         <f t="shared" si="3"/>
         <v>-0.36552028956053351</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>0.12752519531943393</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>-0.19628245268994471</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="6"/>
+        <v>0.71245851941745619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>40339</v>
       </c>
@@ -1008,6 +1069,18 @@
       <c r="N16">
         <f t="shared" si="3"/>
         <v>-0.64694559258574702</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>-0.10762558209160362</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>-0.64694559258574702</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="6"/>
+        <v>0.95336177306970582</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>